<commit_message>
changes to figures, new folder for pdf version of figures
</commit_message>
<xml_diff>
--- a/data/Human_indicators.xlsx
+++ b/data/Human_indicators.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -900,7 +900,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Charcoal</t>
+          <t>Convolvulaceae</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Convolvulaceae</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -910,7 +915,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>high</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -922,17 +927,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Convolvulaceae</t>
+          <t>Cucurbita</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Convolvulaceae</t>
+          <t>Cucurbitaceae</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Indirect</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -942,46 +947,46 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Cucurbita</t>
+          <t>Cyatheaceae</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Cucurbitaceae</t>
+          <t>Cyatheaceae</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Indirect</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>high</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Cyatheaceae</t>
+          <t>Cyperaceae</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Cyatheaceae</t>
+          <t>Cyperaceae</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1003,12 +1008,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Cyperaceae</t>
+          <t>Dodonea</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Cyperaceae</t>
+          <t>Sapindaceae</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1030,17 +1035,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Dodonea</t>
+          <t>Erythroxylum</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Sapindaceae</t>
+          <t>Erythroxylaceae</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Indirect</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1050,24 +1055,24 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Erythroxylum</t>
+          <t>Escallonia resinosa</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Erythroxylaceae</t>
+          <t>Escalloniaceae</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Indirect</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1084,17 +1089,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Escallonia resinosa</t>
+          <t>Eucalyptus</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Escalloniaceae</t>
+          <t>Myrtaceae</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Indirect</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1104,24 +1109,19 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Eucalyptus</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Myrtaceae</t>
+          <t>Gelasinospora</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Indirect</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1138,12 +1138,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Gelasinospora</t>
+          <t>Gossypium</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Malvaceae</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Indirect</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1153,46 +1158,46 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Gossypium</t>
+          <t>Gramineae/Poaceae</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Malvaceae</t>
+          <t>Gramineae/Poaceae</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Indirect</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>low</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Gramineae/Poaceae</t>
+          <t>Grammitis</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Gramineae/Poaceae</t>
+          <t>Polypodiaceae</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1202,7 +1207,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>low</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1214,12 +1219,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Grammitis</t>
+          <t>Heliconia</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Polypodiaceae</t>
+          <t>Helyconiaceae</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1234,19 +1239,19 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Heliconia</t>
+          <t>Juglans</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Helyconiaceae</t>
+          <t>Juglandaceae</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1256,24 +1261,24 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>low</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Juglans</t>
+          <t>Juncaceae</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Juglandaceae</t>
+          <t>Juncaceae</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1283,7 +1288,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>low</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1295,12 +1300,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Juncaceae</t>
+          <t>Lupinus</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Juncaceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1310,7 +1315,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>high</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1322,17 +1327,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Lupinus</t>
+          <t>Manihot</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Fabaceae</t>
+          <t>Euphorbiaceae</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Indirect</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1349,12 +1354,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Manihot</t>
+          <t>Minthostarchys mollis</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Euphorbiaceae</t>
+          <t>Lamiaceae</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1364,51 +1369,51 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>high</t>
+          <t>low</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Minthostarchys mollis</t>
+          <t>Myrica (Morella)</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Lamiaceae</t>
+          <t>Myricaceae</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Indirect</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>low</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Myrica (Morella)</t>
+          <t>Nyctaginaceae</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Myricaceae</t>
+          <t>Nyctaginaceae</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1418,24 +1423,24 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>low</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Nyctaginaceae</t>
+          <t>Oxalidaceae</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Nyctaginaceae</t>
+          <t>Oxalidaceae</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1445,24 +1450,24 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>low</t>
+          <t>high</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Oxalidaceae</t>
+          <t>Passifloraceae</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Oxalidaceae</t>
+          <t>Passifloraceae</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1477,24 +1482,24 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Passifloraceae</t>
+          <t>Persea</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Passifloraceae</t>
+          <t>Lauraceae</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Indirect</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1511,12 +1516,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Persea</t>
+          <t>Phaseolus</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Lauraceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1531,19 +1536,14 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Phaseolus</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Fabaceae</t>
+          <t>Pinus</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1553,7 +1553,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>high</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1565,17 +1565,22 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Pinus</t>
+          <t>Piperaceae</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Piperaceae</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Indirect</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>low</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1587,12 +1592,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Piperaceae</t>
+          <t>Plantago</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Piperaceae</t>
+          <t>Plantaginaceae</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1602,7 +1607,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>low</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1614,12 +1619,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Plantago</t>
+          <t>Polylepis</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Plantaginaceae</t>
+          <t>Rosaceae</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1641,12 +1646,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Polylepis</t>
+          <t>Pouteria lucuma</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Rosaceae</t>
+          <t>Spotaceae</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1656,24 +1661,24 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>high</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Pouteria lucuma</t>
+          <t>Psidium</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Spotaceae</t>
+          <t>Myrtaceae</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1695,12 +1700,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Psidium</t>
+          <t>Pteridaceae</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Myrtaceae</t>
+          <t>Pteridaceae</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1710,24 +1715,24 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>high</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Pteridaceae</t>
+          <t>Rumex</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Pteridaceae</t>
+          <t>Polygonaceae</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1749,12 +1754,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Rumex</t>
+          <t>Sapotaceae</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Polygonaceae</t>
+          <t>Sapotaceae</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1764,7 +1769,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>high</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -1776,12 +1781,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Sapotaceae</t>
+          <t>Schinus molle</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Sapotaceae</t>
+          <t>Anacardiaceae</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1796,19 +1801,19 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Schinus molle</t>
+          <t>Smallanthus</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Anacardiaceae</t>
+          <t>Asteraceae</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1818,7 +1823,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>high</t>
+          <t>low</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -1830,12 +1835,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Smallanthus</t>
+          <t>Solanaceae</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Asteraceae</t>
+          <t>Solanaceae</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1845,24 +1850,24 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>low</t>
+          <t>high</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Solanaceae</t>
+          <t>Spermacoce</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Solanaceae</t>
+          <t>Rubiaceae</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1872,7 +1877,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>high</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -1884,12 +1889,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Spermacoce</t>
+          <t>Sporormiella</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Rubiaceae</t>
+          <t>Sporormiella</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1904,29 +1909,29 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Sporormiella</t>
+          <t>Tropaeolum tuberosum</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Sporormiella</t>
+          <t>Tropaeolaceae</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Indirect</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>high</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -1938,39 +1943,39 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Tropaeolum tuberosum</t>
+          <t>Typhaceae</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Tropaeolaceae</t>
+          <t>Typhaceae</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Indirect</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>high</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Typhaceae</t>
+          <t>Umbelliferae/Apiaceae</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Typhaceae</t>
+          <t>Umbelliferae/Apiaceae</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1980,7 +1985,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>high</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -1992,12 +1997,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Umbelliferae/Apiaceae</t>
+          <t>Urticaceae</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Umbelliferae/Apiaceae</t>
+          <t>Urticaceae</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2007,7 +2012,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>high</t>
+          <t>no</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -2019,22 +2024,22 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Urticaceae</t>
+          <t>Zea mays</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Urticaceae</t>
+          <t>Gramineae</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Indirect</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>high</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2046,17 +2051,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Zea mays</t>
+          <t>Zingiberaceae</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Gramineae</t>
+          <t>Zingiberaceae</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Indirect</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2066,19 +2071,19 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Zingiberaceae</t>
+          <t>Xanthosoma</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Zingiberaceae</t>
+          <t>Araceae</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2089,23 +2094,18 @@
       <c r="D65" t="inlineStr">
         <is>
           <t>high</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>no</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Xanthosoma</t>
+          <t>Dioscorea</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Araceae</t>
+          <t>Dioscoreaceae</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2122,12 +2122,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Dioscorea</t>
+          <t>Anacardiaceae</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Dioscoreaceae</t>
+          <t>Anacardiaceae</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2137,44 +2137,22 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>high</t>
+          <t>low</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Anacardiaceae</t>
+          <t>Fabaceae/Leguminosa</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Anacardiaceae</t>
+          <t>Fabaceae</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
-        <is>
-          <t>Indirect</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>low</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>Fabaceae/Leguminosa</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>Fabaceae</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
         <is>
           <t>Indirect</t>
         </is>

</xml_diff>